<commit_message>
-Act data-raw.R (adapt base nueva) -Act. app.R (pestañas ambiente y trabajo) -Corr peq. app.R (mod. nombres de plot_edu_corte, mod. indicador salud r.png, nombre descargas graficos, etc.)
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -384,396 +384,636 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Derecho</t>
+          <t>Poblacion</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>derecho</t>
+          <t>poblacion</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tipoind</t>
+          <t>Derecho</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>tipoind</t>
+          <t>derecho</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dimensión</t>
+          <t>Tipoind</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dimension</t>
+          <t>tipoind</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Conindicador</t>
+          <t>Dimensión</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>conindicador</t>
+          <t>dimension</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nomindicador</t>
+          <t>Conindicador</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>nomindicador</t>
+          <t>conindicador</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Año</t>
+          <t>Nomindicador</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ano</t>
+          <t>nomindicador</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Fecha cat</t>
+          <t>Año</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>fecha_cat</t>
+          <t>ano</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>Fecha cat</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>valor</t>
+          <t>fecha_cat</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Fuente</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>fuente</t>
+          <t>valor</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Responsable</t>
+          <t>Fuente</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>responsable</t>
+          <t>fuente</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jerarquia</t>
+          <t>Responsable</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>jerarquia</t>
+          <t>responsable</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Corte</t>
+          <t>Jerarquia</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>corte</t>
+          <t>jerarquia</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Corte 2</t>
+          <t>Jerarquia cat</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>corte_2</t>
+          <t>jerarquia_cat</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>Corte</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>nivel</t>
+          <t>corte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Grado</t>
+          <t>Corte 2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>grado</t>
+          <t>corte_2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Categoría de escuela</t>
+          <t>Nivel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>categoria_de_escuela</t>
+          <t>nivel</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Contexto sociocultural de escuela</t>
+          <t>Grado</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>contexto_sociocultural_de_escuela</t>
+          <t>grado</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Asignatura</t>
+          <t>Categoría de escuela</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>asignatura</t>
+          <t>categoria_de_escuela</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tipo de beca educativa</t>
+          <t>Contexto sociocultural de escuela</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>tipo_de_beca_educativa</t>
+          <t>contexto_sociocultural_de_escuela</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Sector</t>
+          <t>Asignatura</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>sector</t>
+          <t>asignatura</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Urbano rural</t>
+          <t>Tipo de beca educativa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>urbano_rural</t>
+          <t>tipo_de_beca_educativa</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Región</t>
+          <t>Sector</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>sector</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Departamento</t>
+          <t>Urbano rural</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>departamento</t>
+          <t>urbano_rural</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Quintil de ingresos</t>
+          <t>Región</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>quintil_de_ingresos</t>
+          <t>region</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Sexo</t>
+          <t>Departamento</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>sexo</t>
+          <t>departamento</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Edad</t>
+          <t>Quintil de ingresos</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>edad</t>
+          <t>quintil_de_ingresos</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Ascendencia étnico-racial</t>
+          <t>Sexo</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ascendencia_etnico_racial</t>
+          <t>sexo</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Pobreza</t>
+          <t>Edad</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>pobreza</t>
+          <t>edad</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Tipo de vacuna</t>
+          <t>Ascendencia étnico-racial</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>tipo_de_vacuna</t>
+          <t>ascendencia_etnico_racial</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Financiamiento</t>
+          <t>Pobreza</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>financiamiento</t>
+          <t>pobreza</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tipo de riesgo</t>
+          <t>Tipo de vacuna</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>tipo_de_riesgo</t>
+          <t>tipo_de_vacuna</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Tipo de solución habitacional</t>
+          <t>Financiamiento</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>tipo_de_solucion_habitacional</t>
+          <t>financiamiento</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>Tipo de riesgo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>tipo_de_riesgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Tipo de solución habitacional</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>tipo_de_solucion_habitacional</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>Prestador</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B37" t="inlineStr">
         <is>
           <t>prestador</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Tipo de vivienda</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>tipo_de_vivienda</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Tipo de instrumento</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>tipo_de_instrumento</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Tipo de inspección</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>tipo_de_inspeccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Tipo de centro</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>tipo_de_centro</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Sector económico</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>sector_economico</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Prevalencia de limitaciones</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>prevalencia_de_limitaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Motivo por el cual se fueron</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>motivo_por_el_cual_se_fueron</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Identidad de género</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>identidad_de_genero</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Área geográfica</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>area_geografica</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Cuenca o embalse</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>cuenca_o_embalse</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Río</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>rio</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Área de capacitación</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>area_de_capacitacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Amparo bse</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>amparo_bse</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Condición migratoria</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>condicion_migratoria</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Adecuación educativa</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>adecuacion_educativa</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Tipo de cláusula</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>tipo_de_clausula</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Causa de muerte</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>causa_de_muerte</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Situación procesal</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>situacion_procesal</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Corr ind ss 310106
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1017,6 +1017,18 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Nota indicador</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>nota_indicador</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
act shiny: 2022, genero, alim, met
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1017,6 +1017,42 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Nivel socioeconómico</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>nivel_socioeconomico</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Tipo de hogar</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>tipo_de_hogar</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Menores en el hogar</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>menores_en_el_hogar</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
act. nota ech y met. gasto
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1053,6 +1053,18 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Metodología mides</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>metodologia_mides</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
act. indicadores edu no ech + género con y sin menores
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -564,12 +564,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Nivel</t>
+          <t>...17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>nivel</t>
+          <t>x17</t>
         </is>
       </c>
     </row>
@@ -1020,12 +1020,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Menores</t>
+          <t>Menores en el hogar</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>menores</t>
+          <t>menores_en_el_hogar</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Act y corr Personas con Discapacidad
</commit_message>
<xml_diff>
--- a/Data/keys.xlsx
+++ b/Data/keys.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1065,6 +1065,54 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Tipo de formación</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>tipo_de_formacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Limitaciones</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>limitaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Tipo de limitación</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>tipo_de_limitacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Necesidades básicas insatisfechas</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>necesidades_basicas_insatisfechas</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>